<commit_message>
added instructions and enable ability
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnoah\AppData\Local\Programs\Python\Python36-32\checkMyNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8672FE45-E475-41B4-A91D-851545297FE0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0F0F48DE-A23E-4836-9715-EAF1B41A8757}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="4284" activeTab="1" xr2:uid="{FEAAD6FF-3F86-42A6-B081-D060BA8B0BED}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
   <si>
     <t>Harvest</t>
   </si>
@@ -68,37 +68,13 @@
     <t>Staff Jones</t>
   </si>
   <si>
-    <t>John left early</t>
-  </si>
-  <si>
-    <t>John left early due to an appt and a doctors appointment he was sick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John was not feeling well.  He had  diarrhea.  Staff called 911 and they broughthim to the Newton ER. </t>
-  </si>
-  <si>
-    <t>Aardvark, Alex</t>
-  </si>
-  <si>
-    <t>Bruno, Bar</t>
-  </si>
-  <si>
-    <t>Clark, Charles</t>
-  </si>
-  <si>
-    <t>Demko, Darren</t>
-  </si>
-  <si>
-    <t>Evelyn, Ema</t>
-  </si>
-  <si>
-    <t>Franklin, Fred</t>
-  </si>
-  <si>
-    <t>Allen, Joe</t>
-  </si>
-  <si>
     <t>Stevens, Rick</t>
+  </si>
+  <si>
+    <t>John was not feeling well.  He had  diarrhea.  This sentence contains the word buttercup exactly one time.</t>
+  </si>
+  <si>
+    <t>John was not feeling well.  He had  diarrhea.  This sentence contains the word  exactly one time.</t>
   </si>
 </sst>
 </file>
@@ -527,7 +503,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,19 +540,17 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43271</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>0.5</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="F2" s="2">
         <v>0.60416666666666663</v>
@@ -593,17 +567,20 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G3">
         <v>16</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43271</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
-        <v>0.60416666666666663</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -614,20 +591,20 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G4">
         <v>17</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43271</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4">
-        <v>15</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -635,22 +612,23 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G5">
         <v>18</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43271</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.60416666666666663</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -661,22 +639,23 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G6">
         <v>19</v>
       </c>
-      <c r="C6" s="1">
-        <v>43271</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="G6">
-        <v>15</v>
+      <c r="H6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -684,19 +663,20 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G7">
         <v>20</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43271</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.30555555555555552</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="G7">
-        <v>15</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
@@ -707,7 +687,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
@@ -720,7 +700,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -728,10 +708,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" t="s">

</xml_diff>